<commit_message>
Updating design to final
</commit_message>
<xml_diff>
--- a/Hardware/Seeed BOM.xlsx
+++ b/Hardware/Seeed BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Designator</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -37,12 +37,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>C1,C2,C7,C10,C16,C17,C18,C19,C20,C21,C22,C23</t>
-  </si>
-  <si>
-    <t>C3,C5,C16</t>
-  </si>
-  <si>
     <t>C4,C6</t>
   </si>
   <si>
@@ -58,24 +52,12 @@
     <t>C12,C13</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
     <t>D3,D4</t>
   </si>
   <si>
-    <t>D5,D6,D7,D8,D9,D10</t>
-  </si>
-  <si>
-    <t>F1,F2</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
@@ -94,9 +76,6 @@
     <t>Q2,Q3</t>
   </si>
   <si>
-    <t>R1,R2,R3,R6,R7,R15,R16,R17,R18,R19</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -112,28 +91,79 @@
     <t>R12</t>
   </si>
   <si>
-    <t>R13,R14,R20</t>
-  </si>
-  <si>
-    <t>R21,R22</t>
-  </si>
-  <si>
     <t>R23</t>
   </si>
   <si>
     <t>R24</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>0402WGF8063TCE</t>
+  </si>
+  <si>
+    <t>RC0402JR-072ML</t>
+  </si>
+  <si>
+    <t>RC0402FR-0747KL</t>
+  </si>
+  <si>
+    <t>RC0402FR-0727RL</t>
+  </si>
+  <si>
+    <t>RC0402JR-071KL</t>
+  </si>
+  <si>
+    <t>RC0402FR-07536KL</t>
+  </si>
+  <si>
+    <t>XC6221A282MR-G</t>
+  </si>
+  <si>
+    <t>PAM2305AABADJ</t>
+  </si>
+  <si>
+    <t>0402WGJ0124TCE</t>
+  </si>
+  <si>
+    <t>C1,C2,C7,C10,C16,C17,C18</t>
+  </si>
+  <si>
+    <t>D5,D6</t>
+  </si>
+  <si>
+    <t>R1,R2,R3,R6,R7,R13,R14,R15,R16,R17,R18,R19,R25</t>
+  </si>
+  <si>
+    <t>C3,C5,C15</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>D1,D12,D13</t>
+  </si>
+  <si>
+    <t>D7,D8,D9,D10,D11</t>
+  </si>
+  <si>
+    <t>R26,R27,R28,R29,R30</t>
+  </si>
+  <si>
+    <t>R20,R31</t>
+  </si>
+  <si>
     <t>SW1</t>
   </si>
   <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>U2</t>
+    <t>U3</t>
   </si>
   <si>
     <t>U4,U5</t>
@@ -145,61 +175,40 @@
     <t>CL05A334KQ5NNNC</t>
   </si>
   <si>
-    <t>1N4148W</t>
-  </si>
-  <si>
-    <t>RC0402JR-0710KL</t>
-  </si>
-  <si>
-    <t>0402WGF8063TCE</t>
-  </si>
-  <si>
-    <t>RC0402JR-072ML</t>
-  </si>
-  <si>
-    <t>RC0402FR-0747KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-0727RL</t>
-  </si>
-  <si>
-    <t>RC0402JR-071KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-0720KL</t>
-  </si>
-  <si>
-    <t>RC0402JR-074K7L</t>
-  </si>
-  <si>
-    <t>RC0402FR-07536KL</t>
-  </si>
-  <si>
-    <t>XC6221A282MR-G</t>
-  </si>
-  <si>
-    <t>PAM2305AABADJ</t>
-  </si>
-  <si>
-    <t>0402WGJ0124TCE</t>
+    <t>1N4148WS</t>
+  </si>
+  <si>
+    <t>19-217/R6C-AL1M2VY/3T</t>
+  </si>
+  <si>
+    <t>RC0402FR-0733RL</t>
+  </si>
+  <si>
+    <t>RC0402JR-0720KL</t>
+  </si>
+  <si>
+    <t>Will send to Seeed</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/CK/JS102011SAQN?qs=%2Fha2pyFaduiwk4yjVSumWwvzELmKSTelN0xiWiCnwb%2F7zmicaddi3A%3D%3D</t>
   </si>
   <si>
     <t>JS102011SAQN</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/c-k/JS102011SAQN/401-1999-1-ND/1640114</t>
-  </si>
-  <si>
-    <t>VL6180X</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/VL6180XV0NR-1/497-14702-1-ND/4854910</t>
-  </si>
-  <si>
-    <t>LM4861</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/texas-instruments/LM4861MX-NOPB/296-38566-2-ND/4090876</t>
+    <t>BMD-340</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/STMicroelectronics/VL6180XV0NR-1?qs=%2Fha2pyFaduhwD2hvgrZYIa%2FLlVtCct%2FN49ZQFrnmgWjTYARAwhiNcX2XT9Yb%2FyTo</t>
+  </si>
+  <si>
+    <t>VL6180XV0NR/1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/LM4861MX-NOPB?qs=%2Fha2pyFadujey1UmQVwE%2FHh0037slp%2FOGNwm%252BDSQHir6q6wRcIxAYQ%3D%3D</t>
+  </si>
+  <si>
+    <t>LM4861MX/NOPB</t>
   </si>
 </sst>
 </file>
@@ -388,13 +397,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
       <color rgb="FF3C3C3C"/>
-      <name val="OpenSans-Semibold"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF3C3C3C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -848,7 +858,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -870,29 +880,26 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1252,13 +1259,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="56" style="5" customWidth="1"/>
@@ -1280,406 +1287,409 @@
     </row>
     <row r="2" spans="1:5" ht="29.1" customHeight="1" thickBot="1">
       <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9">
+        <v>36</v>
+      </c>
+      <c r="B2" s="8">
         <v>302010024</v>
       </c>
-      <c r="C2" s="12">
-        <v>12</v>
+      <c r="C2" s="7">
+        <v>7</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="29.1" customHeight="1" thickBot="1">
-      <c r="A3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8">
         <v>302010003</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="7">
         <v>3</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="29.1" customHeight="1" thickBot="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>302010019</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8">
+        <v>302010171</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
-        <v>302010019</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="B6" s="8">
+        <v>302010005</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8">
+        <v>302010006</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8">
+        <v>302010007</v>
+      </c>
+      <c r="C8" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9">
-        <v>302010171</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9">
-        <v>302010005</v>
-      </c>
-      <c r="C6" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A7" s="8" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="8">
+        <v>304020034</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
-        <v>302010006</v>
-      </c>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A8" s="8" t="s">
+      <c r="B11" s="8">
+        <v>304050003</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9">
-        <v>302010007</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="B12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A9" s="8" t="s">
+    <row r="13" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A10" s="8" t="s">
+      <c r="B14" s="9">
+        <v>320090008</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9">
-        <v>304020034</v>
-      </c>
-      <c r="C10" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A11" s="8" t="s">
+      <c r="B15" s="8">
+        <v>320010000</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="10">
-        <v>304050003</v>
-      </c>
-      <c r="C11" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A12" s="8" t="s">
+      <c r="B16" s="8">
+        <v>320040003</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="B17" s="8">
+        <v>303010114</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9">
+        <v>305030010</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8">
+        <v>305030000</v>
+      </c>
+      <c r="C19" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="9">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A32" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="12">
         <v>304990003</v>
       </c>
-      <c r="C13" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="9">
-        <v>307010159</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="C32" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="12">
-        <v>320090008</v>
-      </c>
-      <c r="C15" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="9">
-        <v>320010000</v>
-      </c>
-      <c r="C16" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="9">
-        <v>320040003</v>
-      </c>
-      <c r="C17" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="9">
-        <v>303010114</v>
-      </c>
-      <c r="C18" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="12">
-        <v>305030010</v>
-      </c>
-      <c r="C19" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="9">
-        <v>305030000</v>
-      </c>
-      <c r="C20" s="12">
+    <row r="33" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A33" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A25" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A26" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A27" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A28" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="13" t="s">
+      <c r="D35" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A36" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A29" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A30" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A31" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="12">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A32" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="9">
-        <v>311130001</v>
-      </c>
-      <c r="C32" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A33" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A34" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A35" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="12">
-        <v>2</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A36" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="12">
+      <c r="B36" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="11">
         <v>1</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
+    <hyperlink ref="D33" r:id="rId1"/>
     <hyperlink ref="D35" r:id="rId2"/>
     <hyperlink ref="D36" r:id="rId3"/>
   </hyperlinks>

</xml_diff>